<commit_message>
made to run based on resourcename and profiles
</commit_message>
<xml_diff>
--- a/src/main/java/utilities/Data.xlsx
+++ b/src/main/java/utilities/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\selenium\eclipse\IPM\src\main\java\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86DC359-522C-44F4-8E97-C9DCB8B70AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB56F1FB-16BF-4915-9B56-3DCD7F6ED444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{55C0C6BC-8E47-487D-8964-ECEE054DEE17}"/>
   </bookViews>
@@ -833,7 +833,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B2" sqref="B2:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Code Changes Done to run in both chrome and firefox
</commit_message>
<xml_diff>
--- a/src/main/java/utilities/Data.xlsx
+++ b/src/main/java/utilities/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\selenium\eclipse\IPM\src\main\java\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB56F1FB-16BF-4915-9B56-3DCD7F6ED444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E8FF1F0-A401-42E8-BDA5-C1C32C2D78A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{55C0C6BC-8E47-487D-8964-ECEE054DEE17}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="144">
   <si>
     <t>Sl.no</t>
   </si>
@@ -458,6 +458,18 @@
   </si>
   <si>
     <t>TestAT6</t>
+  </si>
+  <si>
+    <t>a,b</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>8-6</t>
+  </si>
+  <si>
+    <t>2-4</t>
   </si>
 </sst>
 </file>
@@ -833,7 +845,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F1688C-0C26-4DFF-B71F-83B25D02CB03}">
   <dimension ref="A1:AA14"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:AA14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1252,7 +1264,7 @@
         <v>34</v>
       </c>
       <c r="W3" t="s">
-        <v>18</v>
+        <v>138</v>
       </c>
       <c r="X3" t="s">
         <v>16</v>
@@ -1412,13 +1424,13 @@
         <v>99</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="V5" s="1" t="s">
         <v>34</v>
       </c>
       <c r="W5" t="s">
-        <v>18</v>
+        <v>138</v>
       </c>
       <c r="X5" t="s">
         <v>16</v>
@@ -1430,7 +1442,7 @@
         <v>31</v>
       </c>
       <c r="AA5" t="s">
-        <v>38</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
@@ -1468,25 +1480,25 @@
         <v>12</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>69</v>
+        <v>143</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>74</v>
+        <v>132</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="S6" t="s">
         <v>14</v>
@@ -1495,25 +1507,25 @@
         <v>116</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="V6" s="1" t="s">
         <v>34</v>
       </c>
       <c r="W6" t="s">
-        <v>18</v>
+        <v>138</v>
       </c>
       <c r="X6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="Y6" t="s">
-        <v>22</v>
+        <v>87</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="AA6" t="s">
-        <v>79</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
@@ -1551,7 +1563,7 @@
         <v>12</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>88</v>
+        <v>142</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
assign Remote User condition modified
</commit_message>
<xml_diff>
--- a/src/main/java/utilities/Data.xlsx
+++ b/src/main/java/utilities/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\selenium\eclipse\IPM\src\main\java\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E68246-8097-4677-B8D9-08093B35E284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69166974-BCC7-47F1-8452-97AE7F299F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{55C0C6BC-8E47-487D-8964-ECEE054DEE17}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="147">
   <si>
     <t>Sl.no</t>
   </si>
@@ -470,6 +470,15 @@
   </si>
   <si>
     <t>2-4</t>
+  </si>
+  <si>
+    <t>Windows Server 2022 (Standard Edition without License)</t>
+  </si>
+  <si>
+    <t>10.150.35.0 - akashTest</t>
+  </si>
+  <si>
+    <t>AssignRemoteUser</t>
   </si>
 </sst>
 </file>
@@ -845,7 +854,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,10 +1024,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F1688C-0C26-4DFF-B71F-83B25D02CB03}">
-  <dimension ref="A1:AA14"/>
+  <dimension ref="A1:AB14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="Z13" sqref="Z13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,11 +1035,12 @@
     <col min="2" max="3" width="14.5703125" customWidth="1"/>
     <col min="4" max="4" width="28.28515625" customWidth="1"/>
     <col min="5" max="5" width="23.85546875" customWidth="1"/>
-    <col min="15" max="15" width="17.140625" customWidth="1"/>
+    <col min="15" max="15" width="28.140625" customWidth="1"/>
     <col min="23" max="23" width="21.140625" customWidth="1"/>
+    <col min="24" max="24" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1101,19 +1111,22 @@
         <v>17</v>
       </c>
       <c r="X1" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y1" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1121,19 +1134,19 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>43</v>
+        <v>144</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>28</v>
@@ -1148,10 +1161,10 @@
         <v>12</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>45</v>
+        <v>107</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>45</v>
+        <v>107</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>12</v>
@@ -1160,7 +1173,7 @@
         <v>16</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>27</v>
@@ -1169,34 +1182,37 @@
         <v>13</v>
       </c>
       <c r="S2" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="V2" s="1" t="s">
         <v>34</v>
       </c>
       <c r="W2" t="s">
-        <v>18</v>
+        <v>145</v>
       </c>
       <c r="X2" t="s">
         <v>16</v>
       </c>
       <c r="Y2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z2" t="s">
         <v>22</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1266,20 +1282,20 @@
       <c r="W3" t="s">
         <v>138</v>
       </c>
-      <c r="X3" t="s">
-        <v>16</v>
-      </c>
       <c r="Y3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z3" t="s">
         <v>22</v>
       </c>
-      <c r="Z3" s="1" t="s">
+      <c r="AA3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1349,20 +1365,20 @@
       <c r="W4" t="s">
         <v>18</v>
       </c>
-      <c r="X4" t="s">
-        <v>16</v>
-      </c>
       <c r="Y4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z4" t="s">
         <v>78</v>
       </c>
-      <c r="Z4" s="1" t="s">
+      <c r="AA4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1432,20 +1448,20 @@
       <c r="W5" t="s">
         <v>138</v>
       </c>
-      <c r="X5" t="s">
-        <v>16</v>
-      </c>
       <c r="Y5" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z5" t="s">
         <v>22</v>
       </c>
-      <c r="Z5" s="1" t="s">
+      <c r="AA5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1515,20 +1531,20 @@
       <c r="W6" t="s">
         <v>138</v>
       </c>
-      <c r="X6" t="s">
-        <v>13</v>
-      </c>
       <c r="Y6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z6" t="s">
         <v>87</v>
       </c>
-      <c r="Z6" s="1" t="s">
+      <c r="AA6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1598,20 +1614,20 @@
       <c r="W7" t="s">
         <v>86</v>
       </c>
-      <c r="X7" t="s">
-        <v>13</v>
-      </c>
       <c r="Y7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z7" t="s">
         <v>87</v>
       </c>
-      <c r="Z7" s="1" t="s">
+      <c r="AA7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AB7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1681,20 +1697,20 @@
       <c r="W8" t="s">
         <v>18</v>
       </c>
-      <c r="X8" t="s">
-        <v>13</v>
-      </c>
       <c r="Y8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z8" t="s">
         <v>100</v>
       </c>
-      <c r="Z8" s="1" t="s">
+      <c r="AA8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AB8" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1764,20 +1780,20 @@
       <c r="W9" t="s">
         <v>18</v>
       </c>
-      <c r="X9" t="s">
-        <v>16</v>
-      </c>
       <c r="Y9" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z9" t="s">
         <v>108</v>
       </c>
-      <c r="Z9" s="1" t="s">
+      <c r="AA9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AB9" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1847,20 +1863,20 @@
       <c r="W10" t="s">
         <v>18</v>
       </c>
-      <c r="X10" t="s">
-        <v>16</v>
-      </c>
       <c r="Y10" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z10" t="s">
         <v>108</v>
       </c>
-      <c r="Z10" s="1" t="s">
+      <c r="AA10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="AB10" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1930,20 +1946,20 @@
       <c r="W11" t="s">
         <v>18</v>
       </c>
-      <c r="X11" t="s">
-        <v>16</v>
-      </c>
       <c r="Y11" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z11" t="s">
         <v>108</v>
       </c>
-      <c r="Z11" s="1" t="s">
+      <c r="AA11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AA11" t="s">
+      <c r="AB11" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2013,20 +2029,20 @@
       <c r="W12" t="s">
         <v>126</v>
       </c>
-      <c r="X12" t="s">
-        <v>16</v>
-      </c>
       <c r="Y12" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z12" t="s">
         <v>108</v>
       </c>
-      <c r="Z12" s="1" t="s">
+      <c r="AA12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AA12" t="s">
+      <c r="AB12" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2096,20 +2112,20 @@
       <c r="W13" t="s">
         <v>18</v>
       </c>
-      <c r="X13" t="s">
-        <v>16</v>
-      </c>
       <c r="Y13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z13" t="s">
         <v>108</v>
       </c>
-      <c r="Z13" s="1" t="s">
+      <c r="AA13" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="AA13" t="s">
+      <c r="AB13" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2179,16 +2195,16 @@
       <c r="W14" t="s">
         <v>138</v>
       </c>
-      <c r="X14" t="s">
-        <v>16</v>
-      </c>
       <c r="Y14" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z14" t="s">
         <v>108</v>
       </c>
-      <c r="Z14" s="1" t="s">
+      <c r="AA14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AA14" t="s">
+      <c r="AB14" t="s">
         <v>139</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remote users name check added
</commit_message>
<xml_diff>
--- a/src/main/java/utilities/Data.xlsx
+++ b/src/main/java/utilities/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\selenium\eclipse\IPM\src\main\java\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69166974-BCC7-47F1-8452-97AE7F299F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3A3FCC-B460-498E-99E4-7F9AE12361C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{55C0C6BC-8E47-487D-8964-ECEE054DEE17}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{55C0C6BC-8E47-487D-8964-ECEE054DEE17}"/>
   </bookViews>
   <sheets>
     <sheet name="ResourceName" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="151">
   <si>
     <t>Sl.no</t>
   </si>
@@ -85,9 +85,6 @@
     <t>Daily</t>
   </si>
   <si>
-    <t>3 days</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -169,9 +166,6 @@
     <t>Windows Server</t>
   </si>
   <si>
-    <t>Test_Master_Copy_MC</t>
-  </si>
-  <si>
     <t>vertical</t>
   </si>
   <si>
@@ -479,6 +473,24 @@
   </si>
   <si>
     <t>AssignRemoteUser</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> VCPUS 4 cores, RAM 4 GiB , Disk 32 Gib </t>
+  </si>
+  <si>
+    <t>test1,test2</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>test4</t>
+  </si>
+  <si>
+    <t>lead2=admin,lesad3=user,Pradesep=user</t>
   </si>
 </sst>
 </file>
@@ -878,10 +890,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -889,10 +901,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -900,10 +912,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -911,10 +923,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -922,10 +934,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -933,10 +945,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -944,10 +956,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -955,10 +967,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" t="s">
         <v>101</v>
-      </c>
-      <c r="C9" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -966,10 +978,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" t="s">
         <v>110</v>
-      </c>
-      <c r="C10" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -977,10 +989,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -988,10 +1000,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -999,10 +1011,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1010,10 +1022,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1026,8 +1038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F1688C-0C26-4DFF-B71F-83B25D02CB03}">
   <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z13" sqref="Z13"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3:X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,7 +1063,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
@@ -1063,67 +1075,67 @@
         <v>9</v>
       </c>
       <c r="H1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" t="s">
         <v>64</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>65</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>66</v>
       </c>
-      <c r="M1" t="s">
-        <v>67</v>
-      </c>
-      <c r="N1" t="s">
-        <v>68</v>
-      </c>
       <c r="O1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q1" t="s">
         <v>73</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" t="s">
+        <v>74</v>
+      </c>
+      <c r="T1" t="s">
         <v>75</v>
       </c>
-      <c r="R1" t="s">
-        <v>30</v>
-      </c>
-      <c r="S1" t="s">
-        <v>76</v>
-      </c>
-      <c r="T1" t="s">
-        <v>77</v>
-      </c>
       <c r="U1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V1" t="s">
         <v>35</v>
       </c>
-      <c r="V1" t="s">
-        <v>36</v>
-      </c>
       <c r="W1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="X1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="Y1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z1" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" t="s">
-        <v>21</v>
-      </c>
       <c r="AA1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AB1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -1134,25 +1146,25 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>11</v>
@@ -1161,55 +1173,55 @@
         <v>12</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="S2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="X2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="Y2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Z2" t="s">
-        <v>22</v>
+        <v>150</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AB2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -1223,22 +1235,22 @@
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>11</v>
@@ -1247,22 +1259,22 @@
         <v>12</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>13</v>
@@ -1271,28 +1283,31 @@
         <v>14</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="U3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W3" t="s">
-        <v>138</v>
+        <v>136</v>
+      </c>
+      <c r="X3" t="s">
+        <v>13</v>
       </c>
       <c r="Y3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Z3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AB3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -1306,22 +1321,22 @@
         <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>11</v>
@@ -1330,10 +1345,10 @@
         <v>12</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>11</v>
@@ -1345,37 +1360,40 @@
         <v>13</v>
       </c>
       <c r="Q4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S4" t="s">
+        <v>54</v>
+      </c>
+      <c r="T4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="R4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S4" t="s">
+      <c r="U4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W4" t="s">
+        <v>17</v>
+      </c>
+      <c r="X4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB4" t="s">
         <v>56</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="W4" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -1389,22 +1407,22 @@
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>11</v>
@@ -1413,10 +1431,10 @@
         <v>12</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>11</v>
@@ -1428,7 +1446,7 @@
         <v>13</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>13</v>
@@ -1437,28 +1455,31 @@
         <v>14</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="U5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W5" t="s">
-        <v>138</v>
+        <v>136</v>
+      </c>
+      <c r="X5" t="s">
+        <v>13</v>
       </c>
       <c r="Y5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Z5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -1472,22 +1493,22 @@
         <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>11</v>
@@ -1496,13 +1517,13 @@
         <v>12</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>13</v>
@@ -1511,7 +1532,7 @@
         <v>13</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>13</v>
@@ -1520,28 +1541,31 @@
         <v>14</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="U6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W6" t="s">
+        <v>136</v>
+      </c>
+      <c r="X6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB6" t="s">
         <v>138</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AA6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
@@ -1555,22 +1579,22 @@
         <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>11</v>
@@ -1579,52 +1603,55 @@
         <v>12</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S7" t="s">
+        <v>82</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W7" t="s">
         <v>84</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="X7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z7" t="s">
         <v>85</v>
       </c>
-      <c r="U7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="W7" t="s">
-        <v>86</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>87</v>
-      </c>
       <c r="AA7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AB7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -1635,79 +1662,82 @@
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S8" t="s">
+        <v>54</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="V8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S8" t="s">
-        <v>56</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="W8" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="X8" t="s">
+        <v>13</v>
       </c>
       <c r="Y8" t="s">
         <v>13</v>
       </c>
       <c r="Z8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -1718,28 +1748,28 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="J9" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>12</v>
@@ -1748,7 +1778,7 @@
         <v>12</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>12</v>
@@ -1760,37 +1790,40 @@
         <v>13</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="U9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W9" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="X9" t="s">
+        <v>13</v>
       </c>
       <c r="Y9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Z9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="AA9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
@@ -1801,28 +1834,28 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="J10" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>12</v>
@@ -1831,7 +1864,7 @@
         <v>12</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>12</v>
@@ -1843,37 +1876,40 @@
         <v>13</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="U10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W10" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="X10" t="s">
+        <v>13</v>
       </c>
       <c r="Y10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Z10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
@@ -1884,79 +1920,82 @@
         <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="M11" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="N11" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="S11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W11" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="X11" t="s">
+        <v>13</v>
       </c>
       <c r="Y11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Z11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="AA11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AB11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
@@ -1967,79 +2006,82 @@
         <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="J12" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S12" t="s">
+        <v>82</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W12" t="s">
+        <v>124</v>
+      </c>
+      <c r="X12" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M12" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S12" t="s">
-        <v>84</v>
-      </c>
-      <c r="T12" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="U12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="W12" t="s">
-        <v>126</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>108</v>
-      </c>
-      <c r="AA12" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="AB12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
@@ -2050,40 +2092,40 @@
         <v>8</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="J13" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>13</v>
@@ -2092,37 +2134,40 @@
         <v>13</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="U13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W13" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="X13" t="s">
+        <v>13</v>
       </c>
       <c r="Y13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Z13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="AA13" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AB13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
@@ -2133,40 +2178,40 @@
         <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="J14" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>13</v>
@@ -2175,37 +2220,40 @@
         <v>13</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="S14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="U14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W14" t="s">
-        <v>138</v>
+        <v>136</v>
+      </c>
+      <c r="X14" t="s">
+        <v>13</v>
       </c>
       <c r="Y14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Z14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="AA14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2216,19 +2264,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A629CB-5D60-43E2-9350-568723598546}">
-  <dimension ref="A1:AC14"/>
+  <dimension ref="A1:AD14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Z9" sqref="Z9:Z14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" customWidth="1"/>
+    <col min="10" max="10" width="20" customWidth="1"/>
+    <col min="25" max="25" width="26" customWidth="1"/>
+    <col min="26" max="26" width="17.7109375" customWidth="1"/>
+    <col min="28" max="28" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2245,7 +2302,7 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -2257,99 +2314,102 @@
         <v>9</v>
       </c>
       <c r="J1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" t="s">
         <v>64</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>65</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>66</v>
       </c>
-      <c r="O1" t="s">
-        <v>67</v>
-      </c>
-      <c r="P1" t="s">
-        <v>68</v>
-      </c>
       <c r="Q1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="R1" t="s">
+        <v>71</v>
+      </c>
+      <c r="S1" t="s">
         <v>73</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" t="s">
+        <v>74</v>
+      </c>
+      <c r="V1" t="s">
         <v>75</v>
       </c>
-      <c r="T1" t="s">
-        <v>30</v>
-      </c>
-      <c r="U1" t="s">
-        <v>76</v>
-      </c>
-      <c r="V1" t="s">
-        <v>77</v>
-      </c>
       <c r="W1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X1" t="s">
         <v>35</v>
       </c>
-      <c r="X1" t="s">
-        <v>36</v>
-      </c>
       <c r="Y1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Z1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB1" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>25</v>
-      </c>
       <c r="AC1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>43</v>
+        <v>142</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>11</v>
@@ -2358,63 +2418,66 @@
         <v>12</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="U2" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y2" t="s">
-        <v>18</v>
+        <v>143</v>
       </c>
       <c r="Z2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AA2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
@@ -2423,22 +2486,22 @@
         <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>52</v>
+        <v>145</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>11</v>
@@ -2447,22 +2510,22 @@
         <v>12</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>13</v>
@@ -2471,39 +2534,42 @@
         <v>14</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y3" t="s">
-        <v>18</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="AA3" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
@@ -2512,22 +2578,22 @@
         <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>11</v>
@@ -2536,63 +2602,66 @@
         <v>12</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="O4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U4" t="s">
+        <v>82</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="X4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="P4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="U4" t="s">
-        <v>56</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="Y4" t="s">
-        <v>18</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>16</v>
+        <v>84</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="AA4" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>8</v>
@@ -2601,22 +2670,22 @@
         <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>11</v>
@@ -2625,10 +2694,10 @@
         <v>12</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>11</v>
@@ -2640,7 +2709,7 @@
         <v>13</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>13</v>
@@ -2649,39 +2718,42 @@
         <v>14</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="AA5" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>8</v>
@@ -2690,22 +2762,22 @@
         <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>11</v>
@@ -2714,63 +2786,66 @@
         <v>12</v>
       </c>
       <c r="N6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="P6" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="O6" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="Q6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="U6" t="s">
         <v>14</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Z6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AA6" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>8</v>
@@ -2779,22 +2854,22 @@
         <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>11</v>
@@ -2803,179 +2878,185 @@
         <v>12</v>
       </c>
       <c r="N7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P7" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O7" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="Q7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="U7" t="s">
+        <v>82</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y7" t="s">
         <v>84</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="Z7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB7" t="s">
         <v>85</v>
       </c>
-      <c r="W7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>86</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AC7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="N8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U8" t="s">
+        <v>54</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="X8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="O8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="U8" t="s">
-        <v>56</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="X8" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="Y8" t="s">
-        <v>18</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="AA8" t="s">
-        <v>100</v>
-      </c>
-      <c r="AB8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" t="s">
         <v>101</v>
-      </c>
-      <c r="C9" t="s">
-        <v>103</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>12</v>
@@ -2984,7 +3065,7 @@
         <v>12</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>12</v>
@@ -2996,75 +3077,78 @@
         <v>13</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="U9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="W9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="X9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y9" t="s">
-        <v>18</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="AA9" t="s">
-        <v>108</v>
-      </c>
-      <c r="AB9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" t="s">
         <v>110</v>
-      </c>
-      <c r="C10" t="s">
-        <v>112</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>12</v>
@@ -3073,7 +3157,7 @@
         <v>12</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>12</v>
@@ -3085,354 +3169,366 @@
         <v>13</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="U10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="W10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="X10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y10" t="s">
-        <v>18</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="AA10" t="s">
-        <v>108</v>
-      </c>
-      <c r="AB10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="O11" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="P11" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="U11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y11" t="s">
-        <v>18</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="AA11" t="s">
-        <v>108</v>
-      </c>
-      <c r="AB11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="1" t="s">
+      <c r="I12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U12" t="s">
+        <v>82</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y12" t="s">
         <v>124</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="N12" s="1" t="s">
+      <c r="Z12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O12" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="T12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="U12" t="s">
-        <v>84</v>
-      </c>
-      <c r="V12" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="W12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>126</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>108</v>
-      </c>
-      <c r="AB12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC12" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U13" t="s">
+        <v>82</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="X13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC13" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" t="s">
         <v>23</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="T13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="U13" t="s">
-        <v>84</v>
-      </c>
-      <c r="V13" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="W13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>18</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>108</v>
-      </c>
-      <c r="AB13" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="AC13" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>134</v>
-      </c>
-      <c r="C14" t="s">
-        <v>24</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>137</v>
-      </c>
       <c r="I14" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="L14" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="M14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Q14" s="1" t="s">
         <v>13</v>
@@ -3441,37 +3537,40 @@
         <v>13</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="U14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="W14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="X14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y14" t="s">
-        <v>138</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>16</v>
+        <v>136</v>
+      </c>
+      <c r="Z14" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="AA14" t="s">
-        <v>108</v>
-      </c>
-      <c r="AB14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC14" t="s">
-        <v>139</v>
+        <v>15</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>